<commit_message>
some more pin assignments
</commit_message>
<xml_diff>
--- a/pin assignment.xlsx
+++ b/pin assignment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco\Documents\RAPID-Git\pcbs\rapid_io_module\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ACBB86C-768D-4671-9732-D65ADEC1D24E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5952492-33CA-44FA-B790-B490BC2F8989}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{1C9C7380-D03C-4042-9D8A-EFFEB03C784E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1C9C7380-D03C-4042-9D8A-EFFEB03C784E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="184">
   <si>
     <t>PA0</t>
   </si>
@@ -530,14 +530,71 @@
     <t>COM4_1</t>
   </si>
   <si>
-    <t>CIM4_2</t>
+    <t>COM4_2</t>
+  </si>
+  <si>
+    <t>AIN 1</t>
+  </si>
+  <si>
+    <t>AIN 0</t>
+  </si>
+  <si>
+    <t>ADC 2</t>
+  </si>
+  <si>
+    <t>ADC 3</t>
+  </si>
+  <si>
+    <t>SWCLK</t>
+  </si>
+  <si>
+    <t>SWDIO</t>
+  </si>
+  <si>
+    <t>TH Sense</t>
+  </si>
+  <si>
+    <t>SWITCH</t>
+  </si>
+  <si>
+    <t>SPI_CS_FLASH</t>
+  </si>
+  <si>
+    <t>SWO</t>
+  </si>
+  <si>
+    <t>STAT_LED0</t>
+  </si>
+  <si>
+    <t>STAT_LED1</t>
+  </si>
+  <si>
+    <t>STAT_LED2</t>
+  </si>
+  <si>
+    <t>IO 0</t>
+  </si>
+  <si>
+    <t>IO 1</t>
+  </si>
+  <si>
+    <t>IO 2</t>
+  </si>
+  <si>
+    <t>IO 3</t>
+  </si>
+  <si>
+    <t>IO-3</t>
+  </si>
+  <si>
+    <t>IO-4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -564,6 +621,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="0.39997558519241921"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -585,7 +649,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -608,29 +672,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -668,13 +722,26 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -739,11 +806,11 @@
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{A8A965CF-E602-406D-AA92-4600C141795F}" name="PIN" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{95232349-B929-4EAE-8CA7-E25953754069}" name="NAME" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{51C7EBA4-2120-4BB4-B7EC-353F71F174A6}" name="TYPE (Level)" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{EE382442-C257-4989-A88B-C3420180941A}" name="RAPID" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{06FFD908-E032-49CE-A14C-725C418E8144}" name="Main function after reset" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{2E18468B-8514-4179-A740-5F8008B01ADB}" name="Default" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{5CAA1DE8-748A-4619-B1BF-D318A4B45F4D}" name="Remap" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{51C7EBA4-2120-4BB4-B7EC-353F71F174A6}" name="TYPE (Level)" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{EE382442-C257-4989-A88B-C3420180941A}" name="RAPID" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{06FFD908-E032-49CE-A14C-725C418E8144}" name="Main function after reset" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{2E18468B-8514-4179-A740-5F8008B01ADB}" name="Default" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{5CAA1DE8-748A-4619-B1BF-D318A4B45F4D}" name="Remap" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1068,8 +1135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F60A9F61-B651-48EF-8ADE-300547C97852}">
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D24" sqref="D22:D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1084,7 +1151,7 @@
     <col min="9" max="16384" width="11.5546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>55</v>
       </c>
@@ -1350,7 +1417,9 @@
       <c r="C15" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D15" s="5"/>
+      <c r="D15" s="5" t="s">
+        <v>166</v>
+      </c>
       <c r="E15" s="2" t="s">
         <v>0</v>
       </c>
@@ -1368,7 +1437,9 @@
       <c r="C16" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D16" s="5"/>
+      <c r="D16" s="5" t="s">
+        <v>165</v>
+      </c>
       <c r="E16" s="2" t="s">
         <v>1</v>
       </c>
@@ -1460,7 +1531,9 @@
       <c r="C21" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D21" s="5"/>
+      <c r="D21" s="5" t="s">
+        <v>171</v>
+      </c>
       <c r="E21" s="2" t="s">
         <v>4</v>
       </c>
@@ -1481,9 +1554,7 @@
       <c r="C22" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>148</v>
-      </c>
+      <c r="D22" s="5"/>
       <c r="E22" s="2" t="s">
         <v>5</v>
       </c>
@@ -1501,9 +1572,7 @@
       <c r="C23" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D23" s="5" t="s">
-        <v>149</v>
-      </c>
+      <c r="D23" s="5"/>
       <c r="E23" s="2" t="s">
         <v>6</v>
       </c>
@@ -1524,9 +1593,7 @@
       <c r="C24" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D24" s="5" t="s">
-        <v>150</v>
-      </c>
+      <c r="D24" s="5"/>
       <c r="E24" s="2" t="s">
         <v>7</v>
       </c>
@@ -1547,7 +1614,9 @@
       <c r="C25" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D25" s="5"/>
+      <c r="D25" s="5" t="s">
+        <v>167</v>
+      </c>
       <c r="E25" s="2" t="s">
         <v>36</v>
       </c>
@@ -1565,7 +1634,9 @@
       <c r="C26" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D26" s="5"/>
+      <c r="D26" s="5" t="s">
+        <v>168</v>
+      </c>
       <c r="E26" s="2" t="s">
         <v>37</v>
       </c>
@@ -1767,7 +1838,9 @@
       <c r="C36" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D36" s="5"/>
+      <c r="D36" s="8" t="s">
+        <v>178</v>
+      </c>
       <c r="E36" s="2" t="s">
         <v>30</v>
       </c>
@@ -1785,7 +1858,9 @@
       <c r="C37" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D37" s="5"/>
+      <c r="D37" s="8" t="s">
+        <v>179</v>
+      </c>
       <c r="E37" s="2" t="s">
         <v>31</v>
       </c>
@@ -1803,7 +1878,9 @@
       <c r="C38" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D38" s="5"/>
+      <c r="D38" s="8" t="s">
+        <v>180</v>
+      </c>
       <c r="E38" s="2" t="s">
         <v>38</v>
       </c>
@@ -1824,7 +1901,9 @@
       <c r="C39" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D39" s="5"/>
+      <c r="D39" s="5" t="s">
+        <v>175</v>
+      </c>
       <c r="E39" s="2" t="s">
         <v>39</v>
       </c>
@@ -1845,7 +1924,9 @@
       <c r="C40" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D40" s="5"/>
+      <c r="D40" s="5" t="s">
+        <v>176</v>
+      </c>
       <c r="E40" s="2" t="s">
         <v>40</v>
       </c>
@@ -1864,7 +1945,9 @@
       <c r="C41" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D41" s="5"/>
+      <c r="D41" s="5" t="s">
+        <v>177</v>
+      </c>
       <c r="E41" s="2" t="s">
         <v>41</v>
       </c>
@@ -1923,7 +2006,9 @@
       <c r="C44" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D44" s="5"/>
+      <c r="D44" s="5" t="s">
+        <v>181</v>
+      </c>
       <c r="E44" s="2" t="s">
         <v>10</v>
       </c>
@@ -1981,7 +2066,9 @@
       <c r="C47" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D47" s="5"/>
+      <c r="D47" s="5" t="s">
+        <v>170</v>
+      </c>
       <c r="E47" s="2" t="s">
         <v>105</v>
       </c>
@@ -2034,7 +2121,9 @@
       <c r="C50" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D50" s="5"/>
+      <c r="D50" s="5" t="s">
+        <v>169</v>
+      </c>
       <c r="E50" s="2" t="s">
         <v>115</v>
       </c>
@@ -2052,7 +2141,9 @@
       <c r="C51" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D51" s="5"/>
+      <c r="D51" s="5" t="s">
+        <v>174</v>
+      </c>
       <c r="E51" s="2" t="s">
         <v>116</v>
       </c>
@@ -2119,7 +2210,9 @@
       <c r="C54" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D54" s="5"/>
+      <c r="D54" s="8" t="s">
+        <v>182</v>
+      </c>
       <c r="E54" s="2" t="s">
         <v>44</v>
       </c>
@@ -2140,7 +2233,9 @@
       <c r="C55" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D55" s="5"/>
+      <c r="D55" s="8" t="s">
+        <v>183</v>
+      </c>
       <c r="E55" s="2" t="s">
         <v>48</v>
       </c>
@@ -2158,7 +2253,9 @@
       <c r="C56" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D56" s="5"/>
+      <c r="D56" s="5" t="s">
+        <v>148</v>
+      </c>
       <c r="E56" s="2" t="s">
         <v>125</v>
       </c>
@@ -2179,7 +2276,9 @@
       <c r="C57" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D57" s="5"/>
+      <c r="D57" s="5" t="s">
+        <v>149</v>
+      </c>
       <c r="E57" s="2" t="s">
         <v>126</v>
       </c>
@@ -2200,7 +2299,9 @@
       <c r="C58" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D58" s="5"/>
+      <c r="D58" s="5" t="s">
+        <v>150</v>
+      </c>
       <c r="E58" s="2" t="s">
         <v>21</v>
       </c>
@@ -2284,7 +2385,9 @@
       <c r="C62" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D62" s="5"/>
+      <c r="D62" s="5" t="s">
+        <v>172</v>
+      </c>
       <c r="E62" s="2" t="s">
         <v>24</v>
       </c>
@@ -2305,7 +2408,9 @@
       <c r="C63" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D63" s="5"/>
+      <c r="D63" s="5" t="s">
+        <v>173</v>
+      </c>
       <c r="E63" s="2" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
finished pin assignment, some changes to scematic
</commit_message>
<xml_diff>
--- a/pin assignment.xlsx
+++ b/pin assignment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco\Documents\RAPID-Git\pcbs\rapid_io_module\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5952492-33CA-44FA-B790-B490BC2F8989}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60CBBFC4-6160-4708-80A2-F100AED92B78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1C9C7380-D03C-4042-9D8A-EFFEB03C784E}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{1C9C7380-D03C-4042-9D8A-EFFEB03C784E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="191">
   <si>
     <t>PA0</t>
   </si>
@@ -491,9 +491,6 @@
     <t>SPI1_MOSI</t>
   </si>
   <si>
-    <t>I_sense_main</t>
-  </si>
-  <si>
     <t>v_main_sense</t>
   </si>
   <si>
@@ -539,12 +536,6 @@
     <t>AIN 0</t>
   </si>
   <si>
-    <t>ADC 2</t>
-  </si>
-  <si>
-    <t>ADC 3</t>
-  </si>
-  <si>
     <t>SWCLK</t>
   </si>
   <si>
@@ -572,29 +563,59 @@
     <t>STAT_LED2</t>
   </si>
   <si>
-    <t>IO 0</t>
-  </si>
-  <si>
-    <t>IO 1</t>
-  </si>
-  <si>
-    <t>IO 2</t>
-  </si>
-  <si>
-    <t>IO 3</t>
-  </si>
-  <si>
-    <t>IO-3</t>
-  </si>
-  <si>
-    <t>IO-4</t>
+    <t>I_sense_1</t>
+  </si>
+  <si>
+    <t>I_sense_2</t>
+  </si>
+  <si>
+    <t>AIN 2</t>
+  </si>
+  <si>
+    <t>AIN 3</t>
+  </si>
+  <si>
+    <t>IO-3 (ADC)</t>
+  </si>
+  <si>
+    <t>IO-2 (ADC/DAC)</t>
+  </si>
+  <si>
+    <t>IO-4 (TIM)</t>
+  </si>
+  <si>
+    <t>IO-5</t>
+  </si>
+  <si>
+    <t>IO-6</t>
+  </si>
+  <si>
+    <t>IO-7</t>
+  </si>
+  <si>
+    <t>IO-8</t>
+  </si>
+  <si>
+    <t>IO-9</t>
+  </si>
+  <si>
+    <t>IO-10</t>
+  </si>
+  <si>
+    <t>IO-11</t>
+  </si>
+  <si>
+    <t>IO-0 (UART 5 TX)</t>
+  </si>
+  <si>
+    <t>IO-1 (UART5 RX)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -628,6 +649,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="3" tint="0.499984740745262"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -649,7 +677,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -673,6 +701,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1135,8 +1166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F60A9F61-B651-48EF-8ADE-300547C97852}">
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D24" sqref="D22:D24"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1201,7 +1232,9 @@
       <c r="C3" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D3" s="5"/>
+      <c r="D3" s="9" t="s">
+        <v>185</v>
+      </c>
       <c r="E3" s="2" t="s">
         <v>45</v>
       </c>
@@ -1219,7 +1252,9 @@
       <c r="C4" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D4" s="5"/>
+      <c r="D4" s="9" t="s">
+        <v>186</v>
+      </c>
       <c r="E4" s="2" t="s">
         <v>46</v>
       </c>
@@ -1237,7 +1272,9 @@
       <c r="C5" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D5" s="5"/>
+      <c r="D5" s="9" t="s">
+        <v>187</v>
+      </c>
       <c r="E5" s="2" t="s">
         <v>47</v>
       </c>
@@ -1250,7 +1287,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>112</v>
@@ -1267,7 +1304,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>113</v>
@@ -1303,8 +1340,8 @@
       <c r="C9" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>151</v>
+      <c r="D9" s="9" t="s">
+        <v>179</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>32</v>
@@ -1324,7 +1361,7 @@
         <v>111</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>33</v>
@@ -1344,7 +1381,7 @@
         <v>111</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>34</v>
@@ -1364,7 +1401,7 @@
         <v>111</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>35</v>
@@ -1418,7 +1455,7 @@
         <v>111</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>0</v>
@@ -1438,7 +1475,7 @@
         <v>111</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>1</v>
@@ -1458,7 +1495,7 @@
         <v>111</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>2</v>
@@ -1478,7 +1515,7 @@
         <v>111</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>3</v>
@@ -1532,7 +1569,7 @@
         <v>111</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>4</v>
@@ -1554,7 +1591,9 @@
       <c r="C22" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D22" s="5"/>
+      <c r="D22" s="9" t="s">
+        <v>180</v>
+      </c>
       <c r="E22" s="2" t="s">
         <v>5</v>
       </c>
@@ -1572,7 +1611,9 @@
       <c r="C23" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D23" s="5"/>
+      <c r="D23" s="5" t="s">
+        <v>175</v>
+      </c>
       <c r="E23" s="2" t="s">
         <v>6</v>
       </c>
@@ -1593,7 +1634,9 @@
       <c r="C24" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D24" s="5"/>
+      <c r="D24" s="5" t="s">
+        <v>176</v>
+      </c>
       <c r="E24" s="2" t="s">
         <v>7</v>
       </c>
@@ -1615,7 +1658,7 @@
         <v>111</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>36</v>
@@ -1635,7 +1678,7 @@
         <v>111</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>37</v>
@@ -1700,7 +1743,9 @@
       <c r="C29" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D29" s="5"/>
+      <c r="D29" s="9" t="s">
+        <v>188</v>
+      </c>
       <c r="E29" s="2" t="s">
         <v>18</v>
       </c>
@@ -1719,7 +1764,7 @@
         <v>111</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>26</v>
@@ -1742,7 +1787,7 @@
         <v>111</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>27</v>
@@ -1839,7 +1884,7 @@
         <v>114</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>30</v>
@@ -1859,7 +1904,7 @@
         <v>114</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>31</v>
@@ -1879,7 +1924,7 @@
         <v>114</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>38</v>
@@ -1902,7 +1947,7 @@
         <v>114</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>39</v>
@@ -1925,7 +1970,7 @@
         <v>114</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>40</v>
@@ -1946,7 +1991,7 @@
         <v>114</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>41</v>
@@ -2006,7 +2051,7 @@
       <c r="C44" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D44" s="5" t="s">
+      <c r="D44" s="9" t="s">
         <v>181</v>
       </c>
       <c r="E44" s="2" t="s">
@@ -2067,7 +2112,7 @@
         <v>114</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>105</v>
@@ -2122,7 +2167,7 @@
         <v>114</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>115</v>
@@ -2142,7 +2187,7 @@
         <v>114</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>116</v>
@@ -2165,7 +2210,7 @@
         <v>114</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>42</v>
@@ -2188,7 +2233,7 @@
         <v>114</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>43</v>
@@ -2211,7 +2256,7 @@
         <v>114</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>44</v>
@@ -2234,7 +2279,7 @@
         <v>114</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>48</v>
@@ -2323,7 +2368,7 @@
         <v>114</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>22</v>
@@ -2346,7 +2391,7 @@
         <v>114</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>23</v>
@@ -2386,7 +2431,7 @@
         <v>114</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>24</v>
@@ -2409,7 +2454,7 @@
         <v>114</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
fixed usb and some other issues
</commit_message>
<xml_diff>
--- a/pin assignment.xlsx
+++ b/pin assignment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco\Documents\RAPID-Git\pcbs\rapid_io_module\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60CBBFC4-6160-4708-80A2-F100AED92B78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7F414B-D5C1-40D7-8965-A6754DCC809D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{1C9C7380-D03C-4042-9D8A-EFFEB03C784E}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{1C9C7380-D03C-4042-9D8A-EFFEB03C784E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -461,9 +461,6 @@
     <t>USART1_RTS / OTG_FS_DP / CAN1_TX / TIM1_ETR</t>
   </si>
   <si>
-    <t>RAPID</t>
-  </si>
-  <si>
     <t>USART1_CTS / CAN1_RX / TIM1_CH4/OTG_FS_DM</t>
   </si>
   <si>
@@ -581,9 +578,6 @@
     <t>IO-2 (ADC/DAC)</t>
   </si>
   <si>
-    <t>IO-4 (TIM)</t>
-  </si>
-  <si>
     <t>IO-5</t>
   </si>
   <si>
@@ -596,19 +590,25 @@
     <t>IO-8</t>
   </si>
   <si>
-    <t>IO-9</t>
-  </si>
-  <si>
-    <t>IO-10</t>
-  </si>
-  <si>
-    <t>IO-11</t>
-  </si>
-  <si>
     <t>IO-0 (UART 5 TX)</t>
   </si>
   <si>
     <t>IO-1 (UART5 RX)</t>
+  </si>
+  <si>
+    <t>RAPID IO</t>
+  </si>
+  <si>
+    <t>USB_D-</t>
+  </si>
+  <si>
+    <t>USB_D+</t>
+  </si>
+  <si>
+    <t>USB_FS_VBUS</t>
+  </si>
+  <si>
+    <t>IO-4</t>
   </si>
 </sst>
 </file>
@@ -677,7 +677,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -704,6 +704,15 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -838,7 +847,7 @@
     <tableColumn id="1" xr3:uid="{A8A965CF-E602-406D-AA92-4600C141795F}" name="PIN" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{95232349-B929-4EAE-8CA7-E25953754069}" name="NAME" dataDxfId="5"/>
     <tableColumn id="3" xr3:uid="{51C7EBA4-2120-4BB4-B7EC-353F71F174A6}" name="TYPE (Level)" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{EE382442-C257-4989-A88B-C3420180941A}" name="RAPID" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{EE382442-C257-4989-A88B-C3420180941A}" name="RAPID IO" dataDxfId="3"/>
     <tableColumn id="4" xr3:uid="{06FFD908-E032-49CE-A14C-725C418E8144}" name="Main function after reset" dataDxfId="2"/>
     <tableColumn id="5" xr3:uid="{2E18468B-8514-4179-A740-5F8008B01ADB}" name="Default" dataDxfId="1"/>
     <tableColumn id="6" xr3:uid="{5CAA1DE8-748A-4619-B1BF-D318A4B45F4D}" name="Remap" dataDxfId="0"/>
@@ -1166,8 +1175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F60A9F61-B651-48EF-8ADE-300547C97852}">
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D65" sqref="D65"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1193,7 +1202,7 @@
         <v>109</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>141</v>
+        <v>186</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>106</v>
@@ -1232,8 +1241,8 @@
       <c r="C3" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>185</v>
+      <c r="D3" s="12" t="s">
+        <v>181</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>45</v>
@@ -1253,7 +1262,7 @@
         <v>111</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>46</v>
@@ -1273,7 +1282,7 @@
         <v>111</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>47</v>
@@ -1287,7 +1296,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>112</v>
@@ -1304,7 +1313,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>113</v>
@@ -1341,7 +1350,7 @@
         <v>111</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>32</v>
@@ -1361,7 +1370,7 @@
         <v>111</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>33</v>
@@ -1381,7 +1390,7 @@
         <v>111</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>34</v>
@@ -1401,7 +1410,7 @@
         <v>111</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>35</v>
@@ -1455,7 +1464,7 @@
         <v>111</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>0</v>
@@ -1475,7 +1484,7 @@
         <v>111</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>1</v>
@@ -1495,7 +1504,7 @@
         <v>111</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>2</v>
@@ -1515,7 +1524,7 @@
         <v>111</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>3</v>
@@ -1569,7 +1578,7 @@
         <v>111</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>4</v>
@@ -1592,7 +1601,7 @@
         <v>111</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>5</v>
@@ -1612,7 +1621,7 @@
         <v>111</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>6</v>
@@ -1635,7 +1644,7 @@
         <v>111</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>7</v>
@@ -1658,7 +1667,7 @@
         <v>111</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>36</v>
@@ -1678,7 +1687,7 @@
         <v>111</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>37</v>
@@ -1698,7 +1707,7 @@
         <v>111</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>16</v>
@@ -1721,7 +1730,7 @@
         <v>111</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>17</v>
@@ -1743,8 +1752,8 @@
       <c r="C29" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D29" s="9" t="s">
-        <v>188</v>
+      <c r="D29" s="5" t="s">
+        <v>169</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>18</v>
@@ -1764,7 +1773,7 @@
         <v>111</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>26</v>
@@ -1787,7 +1796,7 @@
         <v>111</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>27</v>
@@ -1884,7 +1893,7 @@
         <v>114</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>30</v>
@@ -1904,7 +1913,7 @@
         <v>114</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>31</v>
@@ -1923,8 +1932,8 @@
       <c r="C38" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D38" s="8" t="s">
-        <v>184</v>
+      <c r="D38" s="10" t="s">
+        <v>168</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>38</v>
@@ -1947,7 +1956,7 @@
         <v>114</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>39</v>
@@ -1970,7 +1979,7 @@
         <v>114</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>40</v>
@@ -1991,7 +2000,7 @@
         <v>114</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>41</v>
@@ -2012,7 +2021,7 @@
         <v>114</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>8</v>
@@ -2032,7 +2041,7 @@
         <v>114</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>146</v>
+        <v>189</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>9</v>
@@ -2051,14 +2060,14 @@
       <c r="C44" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D44" s="9" t="s">
-        <v>181</v>
+      <c r="D44" s="5" t="s">
+        <v>145</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
@@ -2072,13 +2081,13 @@
         <v>114</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>53</v>
+        <v>187</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
@@ -2092,7 +2101,7 @@
         <v>114</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>54</v>
+        <v>188</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>12</v>
@@ -2112,7 +2121,7 @@
         <v>114</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>105</v>
@@ -2167,7 +2176,7 @@
         <v>114</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>115</v>
@@ -2187,7 +2196,7 @@
         <v>114</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>116</v>
@@ -2210,7 +2219,7 @@
         <v>114</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>42</v>
@@ -2233,7 +2242,7 @@
         <v>114</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>43</v>
@@ -2256,7 +2265,7 @@
         <v>114</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>44</v>
@@ -2279,7 +2288,7 @@
         <v>114</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>48</v>
@@ -2299,7 +2308,7 @@
         <v>114</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>125</v>
@@ -2322,7 +2331,7 @@
         <v>114</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>126</v>
@@ -2345,7 +2354,7 @@
         <v>111</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>21</v>
@@ -2368,7 +2377,7 @@
         <v>114</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>22</v>
@@ -2391,7 +2400,7 @@
         <v>114</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>23</v>
@@ -2419,6 +2428,7 @@
       <c r="E61" s="2" t="s">
         <v>50</v>
       </c>
+      <c r="G61" s="11"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
@@ -2431,7 +2441,7 @@
         <v>114</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>169</v>
+        <v>53</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>24</v>
@@ -2439,7 +2449,7 @@
       <c r="F62" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="G62" s="4" t="s">
+      <c r="G62" s="11" t="s">
         <v>138</v>
       </c>
     </row>
@@ -2454,7 +2464,7 @@
         <v>114</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>170</v>
+        <v>54</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>25</v>
@@ -2462,7 +2472,7 @@
       <c r="F63" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="G63" s="4" t="s">
+      <c r="G63" s="11" t="s">
         <v>139</v>
       </c>
     </row>
@@ -2482,6 +2492,7 @@
       <c r="E64" s="2" t="s">
         <v>73</v>
       </c>
+      <c r="G64" s="11"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="1">

</xml_diff>

<commit_message>
started new design iteration, some scematic fixes (servo pwm&5v option, tsv issue)
</commit_message>
<xml_diff>
--- a/pin assignment.xlsx
+++ b/pin assignment.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco\Documents\RAPID-Git\pcbs\rapid_io_module\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7F414B-D5C1-40D7-8965-A6754DCC809D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF3F9B85-9BFE-4810-AFE5-607478B6E840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{1C9C7380-D03C-4042-9D8A-EFFEB03C784E}"/>
   </bookViews>
@@ -38,36 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="191">
   <si>
-    <t>PA0</t>
-  </si>
-  <si>
-    <t>PA1</t>
-  </si>
-  <si>
-    <t>PA2</t>
-  </si>
-  <si>
-    <t>PA3</t>
-  </si>
-  <si>
-    <t>PA4</t>
-  </si>
-  <si>
-    <t>PA5</t>
-  </si>
-  <si>
-    <t>PA6</t>
-  </si>
-  <si>
-    <t>PA7</t>
-  </si>
-  <si>
-    <t>PA8</t>
-  </si>
-  <si>
-    <t>PA9</t>
-  </si>
-  <si>
     <t>PA10</t>
   </si>
   <si>
@@ -86,36 +56,6 @@
     <t>PA15</t>
   </si>
   <si>
-    <t>PB0</t>
-  </si>
-  <si>
-    <t>PB1</t>
-  </si>
-  <si>
-    <t>PB2</t>
-  </si>
-  <si>
-    <t>PB3</t>
-  </si>
-  <si>
-    <t>PB4</t>
-  </si>
-  <si>
-    <t>PB5</t>
-  </si>
-  <si>
-    <t>PB6</t>
-  </si>
-  <si>
-    <t>PB7</t>
-  </si>
-  <si>
-    <t>PB8</t>
-  </si>
-  <si>
-    <t>PB9</t>
-  </si>
-  <si>
     <t>PB10</t>
   </si>
   <si>
@@ -134,36 +74,6 @@
     <t>PB15</t>
   </si>
   <si>
-    <t>PC0</t>
-  </si>
-  <si>
-    <t>PC1</t>
-  </si>
-  <si>
-    <t>PC2</t>
-  </si>
-  <si>
-    <t>PC3</t>
-  </si>
-  <si>
-    <t>PC4</t>
-  </si>
-  <si>
-    <t>PC5</t>
-  </si>
-  <si>
-    <t>PC6</t>
-  </si>
-  <si>
-    <t>PC7</t>
-  </si>
-  <si>
-    <t>PC8</t>
-  </si>
-  <si>
-    <t>PC9</t>
-  </si>
-  <si>
     <t>PC10</t>
   </si>
   <si>
@@ -182,9 +92,6 @@
     <t>PC15</t>
   </si>
   <si>
-    <t>PD2</t>
-  </si>
-  <si>
     <t>NRST</t>
   </si>
   <si>
@@ -497,12 +404,6 @@
     <t>hc2_sense</t>
   </si>
   <si>
-    <t>PD0</t>
-  </si>
-  <si>
-    <t>PD1</t>
-  </si>
-  <si>
     <t>COM1_1</t>
   </si>
   <si>
@@ -527,12 +428,6 @@
     <t>COM4_2</t>
   </si>
   <si>
-    <t>AIN 1</t>
-  </si>
-  <si>
-    <t>AIN 0</t>
-  </si>
-  <si>
     <t>SWCLK</t>
   </si>
   <si>
@@ -572,12 +467,6 @@
     <t>AIN 3</t>
   </si>
   <si>
-    <t>IO-3 (ADC)</t>
-  </si>
-  <si>
-    <t>IO-2 (ADC/DAC)</t>
-  </si>
-  <si>
     <t>IO-5</t>
   </si>
   <si>
@@ -587,9 +476,6 @@
     <t>IO-7</t>
   </si>
   <si>
-    <t>IO-8</t>
-  </si>
-  <si>
     <t>IO-0 (UART 5 TX)</t>
   </si>
   <si>
@@ -609,6 +495,120 @@
   </si>
   <si>
     <t>IO-4</t>
+  </si>
+  <si>
+    <t>PA01</t>
+  </si>
+  <si>
+    <t>PA00</t>
+  </si>
+  <si>
+    <t>PA02</t>
+  </si>
+  <si>
+    <t>PA03</t>
+  </si>
+  <si>
+    <t>PA04</t>
+  </si>
+  <si>
+    <t>PA05</t>
+  </si>
+  <si>
+    <t>PA06</t>
+  </si>
+  <si>
+    <t>PA07</t>
+  </si>
+  <si>
+    <t>PA08</t>
+  </si>
+  <si>
+    <t>PA09</t>
+  </si>
+  <si>
+    <t>PB00</t>
+  </si>
+  <si>
+    <t>PB01</t>
+  </si>
+  <si>
+    <t>PB02</t>
+  </si>
+  <si>
+    <t>PB05</t>
+  </si>
+  <si>
+    <t>PB06</t>
+  </si>
+  <si>
+    <t>PB07</t>
+  </si>
+  <si>
+    <t>PB09</t>
+  </si>
+  <si>
+    <t>PB08</t>
+  </si>
+  <si>
+    <t>PC00</t>
+  </si>
+  <si>
+    <t>PC01</t>
+  </si>
+  <si>
+    <t>PC02</t>
+  </si>
+  <si>
+    <t>PC03</t>
+  </si>
+  <si>
+    <t>PC04</t>
+  </si>
+  <si>
+    <t>PC05</t>
+  </si>
+  <si>
+    <t>PC06</t>
+  </si>
+  <si>
+    <t>PC07</t>
+  </si>
+  <si>
+    <t>PC08</t>
+  </si>
+  <si>
+    <t>PC09</t>
+  </si>
+  <si>
+    <t>AIN_0</t>
+  </si>
+  <si>
+    <t>AIN_1</t>
+  </si>
+  <si>
+    <t>IO_3</t>
+  </si>
+  <si>
+    <t>PD02</t>
+  </si>
+  <si>
+    <t>PD01</t>
+  </si>
+  <si>
+    <t>PD00</t>
+  </si>
+  <si>
+    <t>PB04</t>
+  </si>
+  <si>
+    <t>PB03</t>
+  </si>
+  <si>
+    <t>IO-8 (ADC)</t>
+  </si>
+  <si>
+    <t>IO-2</t>
   </si>
 </sst>
 </file>
@@ -677,7 +677,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -704,15 +704,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -843,6 +834,9 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EFFBDD74-F494-4DE7-B8C9-E19FBF50CFF6}" name="Tabelle2" displayName="Tabelle2" ref="A1:G65" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="A1:G65" xr:uid="{EFFBDD74-F494-4DE7-B8C9-E19FBF50CFF6}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G65">
+    <sortCondition ref="B1:B65"/>
+  </sortState>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{A8A965CF-E602-406D-AA92-4600C141795F}" name="PIN" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{95232349-B929-4EAE-8CA7-E25953754069}" name="NAME" dataDxfId="5"/>
@@ -1175,8 +1169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F60A9F61-B651-48EF-8ADE-300547C97852}">
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1193,1322 +1187,1320 @@
   <sheetData>
     <row r="1" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>56</v>
+        <v>25</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>186</v>
+        <v>148</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>106</v>
+        <v>75</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>69</v>
+        <v>38</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>107</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>57</v>
+        <v>19</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>110</v>
+        <v>81</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>57</v>
+        <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>57</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>181</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>46</v>
+        <v>154</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>182</v>
+        <v>80</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>139</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>46</v>
+        <v>154</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>47</v>
+        <v>153</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>183</v>
+        <v>80</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>140</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>47</v>
+        <v>153</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>58</v>
+        <v>80</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>124</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>59</v>
+        <v>80</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>125</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>59</v>
+        <v>156</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>49</v>
+        <v>157</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>49</v>
+        <v>80</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>32</v>
+        <v>158</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>111</v>
+        <v>80</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>32</v>
+        <v>158</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>33</v>
+        <v>159</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>111</v>
+        <v>80</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>150</v>
+        <v>181</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>33</v>
+        <v>159</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>34</v>
+        <v>160</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>111</v>
+        <v>80</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>151</v>
+        <v>113</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>34</v>
+        <v>160</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>62</v>
+        <v>47</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>35</v>
+        <v>161</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>152</v>
+        <v>114</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>35</v>
+        <v>161</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>64</v>
+        <v>162</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>64</v>
+        <v>83</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>151</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>64</v>
+        <v>162</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>65</v>
+        <v>0</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>44</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="D14" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
-        <v>14</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>157</v>
+        <v>131</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>158</v>
+        <v>130</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>73</v>
+        <v>5</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>73</v>
+        <v>83</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>135</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>73</v>
+        <v>85</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>74</v>
+        <v>163</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>74</v>
+        <v>80</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>112</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>74</v>
+        <v>163</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>4</v>
+        <v>164</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>111</v>
+        <v>80</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>167</v>
+        <v>115</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>4</v>
+        <v>164</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>5</v>
+        <v>165</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>179</v>
+        <v>83</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>134</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>5</v>
+        <v>165</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>6</v>
+        <v>187</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>174</v>
+        <v>117</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>76</v>
+        <v>95</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>96</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>7</v>
+        <v>166</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>111</v>
+        <v>80</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>175</v>
+        <v>118</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>78</v>
+        <v>166</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>100</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>36</v>
+        <v>167</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>176</v>
+        <v>122</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>82</v>
+        <v>167</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>37</v>
+        <v>168</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>177</v>
+        <v>123</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>83</v>
+        <v>168</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>16</v>
+        <v>170</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>143</v>
+        <v>22</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>84</v>
+        <v>170</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>106</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>86</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>17</v>
+        <v>169</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>146</v>
+        <v>23</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>85</v>
+        <v>169</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>108</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>169</v>
+        <v>126</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>111</v>
+        <v>80</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>159</v>
+        <v>127</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>90</v>
+        <v>61</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>160</v>
+        <v>21</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>73</v>
+        <v>9</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>73</v>
+        <v>83</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>73</v>
+        <v>9</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>74</v>
+        <v>10</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>74</v>
+        <v>83</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>152</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>52</v>
+        <v>83</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>143</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>29</v>
+        <v>188</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>114</v>
+        <v>83</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>51</v>
+        <v>116</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F35" s="2" t="s">
         <v>94</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>30</v>
+        <v>171</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>190</v>
+        <v>80</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>189</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>30</v>
+        <v>171</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>95</v>
+        <v>29</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>31</v>
+        <v>172</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>180</v>
+        <v>80</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>119</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>31</v>
+        <v>172</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>96</v>
+        <v>30</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>38</v>
+        <v>173</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D38" s="10" t="s">
-        <v>168</v>
+        <v>80</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>120</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>38</v>
+        <v>173</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="G38" s="4" t="s">
-        <v>98</v>
+        <v>31</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>39</v>
+        <v>174</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>171</v>
+        <v>121</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>39</v>
+        <v>174</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="G39" s="4" t="s">
-        <v>100</v>
+        <v>32</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>40</v>
+        <v>175</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>172</v>
+        <v>142</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2" t="s">
-        <v>101</v>
+        <v>175</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>41</v>
+        <v>176</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>173</v>
+        <v>141</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F41" s="2"/>
-      <c r="G41" s="4" t="s">
-        <v>102</v>
+        <v>176</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>8</v>
+        <v>177</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>114</v>
+        <v>83</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>8</v>
+        <v>177</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>103</v>
+        <v>66</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>9</v>
+        <v>178</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>114</v>
+        <v>83</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>189</v>
+        <v>136</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>9</v>
+        <v>178</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>104</v>
+        <v>68</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>10</v>
+        <v>179</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>114</v>
+        <v>83</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>142</v>
+        <v>179</v>
+      </c>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>11</v>
+        <v>180</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>114</v>
+        <v>83</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>187</v>
+        <v>138</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+        <v>180</v>
+      </c>
+      <c r="F45" s="2"/>
+      <c r="G45" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>114</v>
+        <v>83</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>188</v>
+        <v>128</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F46" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F46" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>114</v>
+        <v>83</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>166</v>
+        <v>129</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="F47" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>90</v>
+      </c>
       <c r="G47" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A48" s="1">
+        <v>53</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" s="1">
+        <v>2</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" s="1">
+        <v>3</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" s="1">
+        <v>4</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" s="1">
+        <v>5</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D52" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" s="1">
+        <v>6</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" s="1">
+        <v>54</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" s="1">
+        <v>1</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" s="1">
+        <v>19</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" s="1">
+        <v>32</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" s="1">
+        <v>48</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" s="1">
+        <v>64</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" s="1">
         <v>13</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="1">
+      <c r="B60" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" s="1">
+        <v>18</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" s="1">
+        <v>31</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" s="1">
         <v>47</v>
       </c>
-      <c r="B48" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="1">
-        <v>48</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D49" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="1">
-        <v>49</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="G50" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A51" s="1">
-        <v>50</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="F51" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="G51" s="4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A52" s="1">
-        <v>51</v>
-      </c>
-      <c r="B52" s="2" t="s">
+      <c r="B63" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C52" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="E52" s="2" t="s">
+      <c r="C63" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D63" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F52" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="G52" s="4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A53" s="1">
-        <v>52</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F53" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="G53" s="4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A54" s="1">
-        <v>53</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D54" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F54" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="G54" s="4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A55" s="1">
-        <v>54</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D55" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F55" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A56" s="1">
-        <v>55</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="F56" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="G56" s="4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A57" s="1">
-        <v>56</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="F57" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="G57" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A58" s="1">
-        <v>57</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F58" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="G58" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A59" s="1">
-        <v>58</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F59" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="G59" s="4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A60" s="1">
-        <v>59</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D60" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F60" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="G60" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A61" s="1">
-        <v>60</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="D61" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G61" s="11"/>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A62" s="1">
-        <v>61</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D62" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F62" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="G62" s="11" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A63" s="1">
-        <v>62</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D63" s="5" t="s">
-        <v>54</v>
-      </c>
       <c r="E63" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F63" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="G63" s="11" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>63</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>110</v>
+        <v>79</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="G64" s="11"/>
+        <v>42</v>
+      </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
-        <v>64</v>
+        <v>12</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>74</v>
+        <v>33</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>110</v>
+        <v>79</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>74</v>
+        <v>33</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>74</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>